<commit_message>
correccion nombre columna excel crr por crr2
</commit_message>
<xml_diff>
--- a/data/pds.xlsx
+++ b/data/pds.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -146,7 +146,7 @@
     <t>tertiary</t>
   </si>
   <si>
-    <t>CRR</t>
+    <t>CRR2</t>
   </si>
 </sst>
 </file>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>